<commit_message>
New codesets generated using codeset generator M.Hancock
</commit_message>
<xml_diff>
--- a/xlsx/organisation-type.xlsx
+++ b/xlsx/organisation-type.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -26,6 +26,9 @@
     <t xml:space="preserve">Definition</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.0</t>
   </si>
   <si>
@@ -36,6 +39,9 @@
   </si>
   <si>
     <t xml:space="preserve">Public service departments, non-public service departments, offices of Parliament and the Reserve Bank of NZ. State Sector Act 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic</t>
   </si>
   <si>
     <t xml:space="preserve">DA02</t>
@@ -185,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">Any government, state entity or local authority of another country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International</t>
   </si>
   <si>
     <t xml:space="preserve">IG01</t>
@@ -559,235 +568,289 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5"/>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6"/>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12"/>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D15"/>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>